<commit_message>
update LAOs results and block speed-up during tests
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Discounted cash flow.xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Discounted cash flow.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{70E65E1C-B69D-4A64-B936-73550718AC0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{698DBD12-8861-4192-B763-337C75053E4A}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{70E65E1C-B69D-4A64-B936-73550718AC0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F3DDC662-2558-475A-A659-CFE242C3A37A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tables S49-S50" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables S52-S53" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,10 +78,10 @@
     <t>Cumilative NPV [MM$]</t>
   </si>
   <si>
-    <t>Table S50. Discounted cash flow analysis of the production process at the present-day fermentation performance scenario.</t>
+    <t>Table S52. Discounted cash flow analysis of the production process at the baseline fermentation performance scenario.</t>
   </si>
   <si>
-    <t>Table S51. Discounted cash flow analysis of the production process at the present-day fermentation performance scenario.</t>
+    <t>Table S53. Discounted cash flow analysis of the production process at the target fermentation performance scenario.</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>